<commit_message>
new files,CLI spaCy, README
</commit_message>
<xml_diff>
--- a/JupyterNoteBook/table_savoirs.xlsx
+++ b/JupyterNoteBook/table_savoirs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexsoares/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexsoares/Desktop/EHESS/dev/Savoirs_env/JupyterNoteBook/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
   <si>
     <t>db_savoirs/BNU_01_Didier.xml</t>
   </si>
@@ -323,9 +323,6 @@
     <t>db_savoirs/LDSII_52_Kassow_OnegShabbes.xml</t>
   </si>
   <si>
-    <t>​</t>
-  </si>
-  <si>
     <t>Database_Savoirs</t>
   </si>
   <si>
@@ -339,6 +336,12 @@
   </si>
   <si>
     <t>Total_mots</t>
+  </si>
+  <si>
+    <t>Total_ENT</t>
+  </si>
+  <si>
+    <t>Total =</t>
   </si>
 </sst>
 </file>
@@ -662,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D103"/>
+  <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="E104" sqref="E104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -673,29 +676,32 @@
     <col min="1" max="1" width="41.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" t="s">
         <v>102</v>
       </c>
-      <c r="B2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -708,8 +714,12 @@
       <c r="D4" s="1">
         <v>3880</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <f>B4+C4</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -722,8 +732,12 @@
       <c r="D5" s="1">
         <v>24791</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <f t="shared" ref="E5:E68" si="0">B5+C5</f>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -736,8 +750,12 @@
       <c r="D6" s="1">
         <v>5928</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -750,8 +768,12 @@
       <c r="D7" s="1">
         <v>5125</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -764,8 +786,12 @@
       <c r="D8" s="1">
         <v>5633</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -778,8 +804,12 @@
       <c r="D9" s="1">
         <v>1928</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -792,8 +822,12 @@
       <c r="D10" s="1">
         <v>7030</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -806,8 +840,12 @@
       <c r="D11" s="1">
         <v>7208</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -820,8 +858,12 @@
       <c r="D12" s="1">
         <v>9284</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -834,8 +876,12 @@
       <c r="D13" s="1">
         <v>4250</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -848,8 +894,12 @@
       <c r="D14" s="1">
         <v>7102</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -862,8 +912,12 @@
       <c r="D15" s="1">
         <v>6394</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -876,8 +930,12 @@
       <c r="D16" s="1">
         <v>8752</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -890,8 +948,12 @@
       <c r="D17" s="1">
         <v>13176</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -904,8 +966,12 @@
       <c r="D18" s="1">
         <v>8070</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
@@ -918,8 +984,12 @@
       <c r="D19" s="1">
         <v>6088</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
@@ -932,8 +1002,12 @@
       <c r="D20" s="1">
         <v>7362</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
@@ -946,8 +1020,12 @@
       <c r="D21" s="1">
         <v>8452</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
@@ -960,8 +1038,12 @@
       <c r="D22" s="1">
         <v>9148</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -974,8 +1056,12 @@
       <c r="D23" s="1">
         <v>6950</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
@@ -988,8 +1074,12 @@
       <c r="D24" s="1">
         <v>14464</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
@@ -1002,8 +1092,12 @@
       <c r="D25" s="1">
         <v>11786</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
@@ -1016,8 +1110,12 @@
       <c r="D26" s="1">
         <v>14758</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
@@ -1030,8 +1128,12 @@
       <c r="D27" s="1">
         <v>19144</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
@@ -1044,8 +1146,12 @@
       <c r="D28" s="1">
         <v>11878</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -1058,8 +1164,12 @@
       <c r="D29" s="1">
         <v>10654</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>26</v>
       </c>
@@ -1072,8 +1182,12 @@
       <c r="D30" s="1">
         <v>9146</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>27</v>
       </c>
@@ -1086,8 +1200,12 @@
       <c r="D31" s="1">
         <v>3930</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>28</v>
       </c>
@@ -1100,8 +1218,12 @@
       <c r="D32" s="1">
         <v>15228</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
@@ -1114,8 +1236,12 @@
       <c r="D33" s="1">
         <v>2958</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>30</v>
       </c>
@@ -1128,8 +1254,12 @@
       <c r="D34" s="1">
         <v>16330</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>31</v>
       </c>
@@ -1142,8 +1272,12 @@
       <c r="D35" s="1">
         <v>6442</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>32</v>
       </c>
@@ -1156,8 +1290,12 @@
       <c r="D36" s="1">
         <v>15969</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>33</v>
       </c>
@@ -1170,8 +1308,12 @@
       <c r="D37" s="1">
         <v>15144</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>34</v>
       </c>
@@ -1184,8 +1326,12 @@
       <c r="D38" s="1">
         <v>5580</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>35</v>
       </c>
@@ -1198,8 +1344,12 @@
       <c r="D39" s="1">
         <v>11839</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>36</v>
       </c>
@@ -1212,8 +1362,12 @@
       <c r="D40" s="1">
         <v>14328</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>37</v>
       </c>
@@ -1226,8 +1380,12 @@
       <c r="D41" s="1">
         <v>13930</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>38</v>
       </c>
@@ -1240,8 +1398,12 @@
       <c r="D42" s="1">
         <v>3658</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>39</v>
       </c>
@@ -1254,8 +1416,12 @@
       <c r="D43" s="1">
         <v>14204</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>40</v>
       </c>
@@ -1268,8 +1434,12 @@
       <c r="D44" s="1">
         <v>14326</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>41</v>
       </c>
@@ -1282,8 +1452,12 @@
       <c r="D45" s="1">
         <v>16272</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>42</v>
       </c>
@@ -1296,8 +1470,12 @@
       <c r="D46" s="1">
         <v>5488</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>43</v>
       </c>
@@ -1310,8 +1488,12 @@
       <c r="D47" s="1">
         <v>14264</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>290</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>44</v>
       </c>
@@ -1324,8 +1506,12 @@
       <c r="D48" s="1">
         <v>13510</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>45</v>
       </c>
@@ -1338,8 +1524,12 @@
       <c r="D49" s="1">
         <v>13948</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <f t="shared" si="0"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>46</v>
       </c>
@@ -1352,8 +1542,12 @@
       <c r="D50" s="1">
         <v>12402</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>47</v>
       </c>
@@ -1366,8 +1560,12 @@
       <c r="D51" s="1">
         <v>5658</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>48</v>
       </c>
@@ -1380,8 +1578,12 @@
       <c r="D52" s="1">
         <v>14888</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <f t="shared" si="0"/>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>49</v>
       </c>
@@ -1394,8 +1596,12 @@
       <c r="D53" s="1">
         <v>4454</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E53">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>50</v>
       </c>
@@ -1408,8 +1614,12 @@
       <c r="D54" s="1">
         <v>15100</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E54">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>51</v>
       </c>
@@ -1422,8 +1632,12 @@
       <c r="D55" s="1">
         <v>6144</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E55">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>52</v>
       </c>
@@ -1436,8 +1650,12 @@
       <c r="D56" s="1">
         <v>17364</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E56">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>53</v>
       </c>
@@ -1450,8 +1668,12 @@
       <c r="D57" s="1">
         <v>7006</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E57">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>54</v>
       </c>
@@ -1464,8 +1686,12 @@
       <c r="D58" s="1">
         <v>11550</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E58">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>55</v>
       </c>
@@ -1478,8 +1704,12 @@
       <c r="D59" s="1">
         <v>9897</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E59">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>56</v>
       </c>
@@ -1492,8 +1722,12 @@
       <c r="D60" s="1">
         <v>11648</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E60">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>57</v>
       </c>
@@ -1506,8 +1740,12 @@
       <c r="D61" s="1">
         <v>5378</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E61">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>58</v>
       </c>
@@ -1520,8 +1758,12 @@
       <c r="D62" s="1">
         <v>4803</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E62">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>59</v>
       </c>
@@ -1534,8 +1776,12 @@
       <c r="D63" s="1">
         <v>15624</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E63">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>60</v>
       </c>
@@ -1548,8 +1794,12 @@
       <c r="D64" s="1">
         <v>14648</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E64">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>61</v>
       </c>
@@ -1562,8 +1812,12 @@
       <c r="D65" s="1">
         <v>14486</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>62</v>
       </c>
@@ -1576,8 +1830,12 @@
       <c r="D66" s="1">
         <v>7802</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E66">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>63</v>
       </c>
@@ -1590,8 +1848,12 @@
       <c r="D67" s="1">
         <v>12452</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E67">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>64</v>
       </c>
@@ -1604,8 +1866,12 @@
       <c r="D68" s="1">
         <v>16818</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E68">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>65</v>
       </c>
@@ -1618,8 +1884,12 @@
       <c r="D69" s="1">
         <v>11362</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E69">
+        <f t="shared" ref="E69:E101" si="1">B69+C69</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>66</v>
       </c>
@@ -1632,8 +1902,12 @@
       <c r="D70" s="1">
         <v>12724</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E70">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>67</v>
       </c>
@@ -1646,8 +1920,12 @@
       <c r="D71" s="1">
         <v>5030</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E71">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>68</v>
       </c>
@@ -1660,8 +1938,12 @@
       <c r="D72" s="1">
         <v>14580</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E72">
+        <f t="shared" si="1"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>69</v>
       </c>
@@ -1674,8 +1956,12 @@
       <c r="D73" s="1">
         <v>14824</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E73">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>70</v>
       </c>
@@ -1688,8 +1974,12 @@
       <c r="D74" s="1">
         <v>13028</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E74">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>71</v>
       </c>
@@ -1702,8 +1992,12 @@
       <c r="D75" s="1">
         <v>13924</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E75">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>72</v>
       </c>
@@ -1716,8 +2010,12 @@
       <c r="D76" s="1">
         <v>5718</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E76">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>73</v>
       </c>
@@ -1730,8 +2028,12 @@
       <c r="D77" s="1">
         <v>13326</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E77">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>74</v>
       </c>
@@ -1744,8 +2046,12 @@
       <c r="D78" s="1">
         <v>12196</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E78">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>75</v>
       </c>
@@ -1758,8 +2064,12 @@
       <c r="D79" s="1">
         <v>6424</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E79">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>76</v>
       </c>
@@ -1772,8 +2082,12 @@
       <c r="D80" s="1">
         <v>13469</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E80">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>77</v>
       </c>
@@ -1786,8 +2100,12 @@
       <c r="D81" s="1">
         <v>17192</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E81">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>78</v>
       </c>
@@ -1800,8 +2118,12 @@
       <c r="D82" s="1">
         <v>8970</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E82">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>79</v>
       </c>
@@ -1814,8 +2136,12 @@
       <c r="D83" s="1">
         <v>10256</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E83">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>80</v>
       </c>
@@ -1828,8 +2154,12 @@
       <c r="D84" s="1">
         <v>15260</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E84">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>81</v>
       </c>
@@ -1842,8 +2172,12 @@
       <c r="D85" s="1">
         <v>6022</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E85">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>82</v>
       </c>
@@ -1856,8 +2190,12 @@
       <c r="D86" s="1">
         <v>13396</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E86">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>83</v>
       </c>
@@ -1870,8 +2208,12 @@
       <c r="D87" s="1">
         <v>18698</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E87">
+        <f t="shared" si="1"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>84</v>
       </c>
@@ -1884,8 +2226,12 @@
       <c r="D88" s="1">
         <v>13926</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E88">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>85</v>
       </c>
@@ -1898,8 +2244,12 @@
       <c r="D89" s="1">
         <v>13445</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E89">
+        <f t="shared" si="1"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>86</v>
       </c>
@@ -1912,8 +2262,12 @@
       <c r="D90" s="1">
         <v>15971</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E90">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>87</v>
       </c>
@@ -1926,8 +2280,12 @@
       <c r="D91" s="1">
         <v>15070</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E91">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>88</v>
       </c>
@@ -1940,8 +2298,12 @@
       <c r="D92" s="1">
         <v>4970</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E92">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>89</v>
       </c>
@@ -1954,8 +2316,12 @@
       <c r="D93" s="1">
         <v>12997</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E93">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>90</v>
       </c>
@@ -1968,8 +2334,12 @@
       <c r="D94" s="1">
         <v>16641</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E94">
+        <f t="shared" si="1"/>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>91</v>
       </c>
@@ -1982,8 +2352,12 @@
       <c r="D95" s="1">
         <v>8716</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E95">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>92</v>
       </c>
@@ -1996,8 +2370,12 @@
       <c r="D96" s="1">
         <v>6030</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E96">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>93</v>
       </c>
@@ -2010,8 +2388,12 @@
       <c r="D97" s="1">
         <v>9284</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E97">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>94</v>
       </c>
@@ -2024,8 +2406,12 @@
       <c r="D98" s="1">
         <v>13152</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E98">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>95</v>
       </c>
@@ -2038,8 +2424,12 @@
       <c r="D99" s="1">
         <v>13449</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E99">
+        <f t="shared" si="1"/>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>96</v>
       </c>
@@ -2052,8 +2442,12 @@
       <c r="D100" s="1">
         <v>8890</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E100">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>97</v>
       </c>
@@ -2066,10 +2460,30 @@
       <c r="D101" s="1">
         <v>19698</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E101">
+        <f t="shared" si="1"/>
+        <v>266</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>98</v>
+        <v>104</v>
+      </c>
+      <c r="B103">
+        <f xml:space="preserve"> SUM(B4:B101)</f>
+        <v>1651</v>
+      </c>
+      <c r="C103">
+        <f t="shared" ref="C103:E103" si="2" xml:space="preserve"> SUM(C4:C101)</f>
+        <v>4974</v>
+      </c>
+      <c r="D103">
+        <f t="shared" si="2"/>
+        <v>1072489</v>
+      </c>
+      <c r="E103">
+        <f xml:space="preserve"> SUM(B103+C103)</f>
+        <v>6625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>